<commit_message>
Correct a few mistakes in import.
</commit_message>
<xml_diff>
--- a/database/imports/game/Abilities.xlsx
+++ b/database/imports/game/Abilities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\oliver\dbgt\database\imports\game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B512EC3A-D5B0-4415-9455-47CFF4E16CF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEE98DD-27AC-4249-8F92-42DE5D44F9AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19020" yWindow="4530" windowWidth="18640" windowHeight="13520" xr2:uid="{927729A4-4100-4AD3-9E50-E6FD35BB57B8}"/>
+    <workbookView xWindow="12910" yWindow="470" windowWidth="28590" windowHeight="17700" activeTab="1" xr2:uid="{927729A4-4100-4AD3-9E50-E6FD35BB57B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Abilities" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="96">
   <si>
     <t>NAME</t>
   </si>
@@ -205,9 +205,6 @@
     <t>DEATH_SAUCER</t>
   </si>
   <si>
-    <t>SPECAL</t>
-  </si>
-  <si>
     <t>An energy weapon in the shape of a sharp, spinning disc. Incredibly fast and has a chance to OHKO.</t>
   </si>
   <si>
@@ -292,27 +289,15 @@
     <t>TIEN</t>
   </si>
   <si>
-    <t>FINAL_FORM_FRIEZA</t>
-  </si>
-  <si>
     <t>FIGHTER CODES</t>
   </si>
   <si>
-    <t>GOKU,KRILLIN,TIEN</t>
-  </si>
-  <si>
     <t>KING_PICCOLO</t>
   </si>
   <si>
     <t>KID_GOKU</t>
   </si>
   <si>
-    <t>GOKU,GOKU_SUPER_SAIYAN,GOKU_KAIOKEN</t>
-  </si>
-  <si>
-    <t>FRIEZA,FRIEZA_SECOND_FORM,FRIEZA_THIRD_FORM</t>
-  </si>
-  <si>
     <t>Impale</t>
   </si>
   <si>
@@ -325,7 +310,19 @@
     <t>FRIEZA_SECOND_FORM</t>
   </si>
   <si>
-    <t>KRILLIN;KID_GOKU;GOKU_SUPER_SAIYAN,GOKU_KAIOKEN</t>
+    <t>KRILLIN;KID_GOKU;GOKU_SUPER_SAIYAN;GOKU_KAIOKEN</t>
+  </si>
+  <si>
+    <t>FRIEZA;FRIEZA_SECOND_FORM;FRIEZA_THIRD_FORM</t>
+  </si>
+  <si>
+    <t>GOKU;GOKU_SUPER_SAIYAN;GOKU_KAIOKEN</t>
+  </si>
+  <si>
+    <t>GOKU;KRILLIN;TIEN</t>
+  </si>
+  <si>
+    <t>FRIEZA_FINAL_FORM</t>
   </si>
 </sst>
 </file>
@@ -409,11 +406,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDB0151-4FC2-40F8-8BF2-9DFDBC6AD7A6}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -745,13 +742,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="32.5" x14ac:dyDescent="0.65">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1027,10 +1024,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1">
         <v>8</v>
@@ -1039,7 +1036,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1053,18 +1050,18 @@
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C20" s="1">
         <v>30</v>
@@ -1073,15 +1070,15 @@
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
@@ -1090,15 +1087,15 @@
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C22" s="1">
         <v>10</v>
@@ -1107,15 +1104,15 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
@@ -1124,15 +1121,15 @@
         <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -1141,15 +1138,15 @@
         <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C25" s="1">
         <v>20</v>
@@ -1158,15 +1155,15 @@
         <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C26" s="1">
         <v>10</v>
@@ -1175,7 +1172,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1191,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A66644-8897-4082-8882-84939572C075}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1203,17 +1200,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="32.5" x14ac:dyDescent="0.65">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>86</v>
+      <c r="A2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1221,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1229,7 +1226,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1237,7 +1234,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1245,7 +1242,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1253,7 +1250,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1261,7 +1258,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1269,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1277,7 +1274,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1285,7 +1282,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1293,7 +1290,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1301,7 +1298,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -1309,7 +1306,7 @@
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -1317,7 +1314,7 @@
         <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -1325,7 +1322,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1333,15 +1330,15 @@
         <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1349,62 +1346,64 @@
         <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>